<commit_message>
maj nom tbl JE
</commit_message>
<xml_diff>
--- a/Sprint 1/Package 1/Documentation/P01_JE_V2.xlsx
+++ b/Sprint 1/Package 1/Documentation/P01_JE_V2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="12228" yWindow="12" windowWidth="10800" windowHeight="9348" tabRatio="861" activeTab="1"/>
+    <workbookView xWindow="12228" yWindow="12" windowWidth="10800" windowHeight="9348" tabRatio="861" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="C tblSysExp" sheetId="3" r:id="rId1"/>
@@ -17,8 +17,8 @@
     <sheet name="B tblJeu" sheetId="6" r:id="rId8"/>
     <sheet name="C tblPlateformeSysExp" sheetId="16" r:id="rId9"/>
     <sheet name="B tblThemeJeu" sheetId="7" r:id="rId10"/>
-    <sheet name="tblVersion" sheetId="10" r:id="rId11"/>
-    <sheet name="tblJeuSemblable" sheetId="12" r:id="rId12"/>
+    <sheet name="B tblVersion" sheetId="10" r:id="rId11"/>
+    <sheet name="B tblJeuSemblable" sheetId="12" r:id="rId12"/>
     <sheet name="B tblPlateformeJeu" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1181" uniqueCount="819">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1182" uniqueCount="820">
   <si>
     <t>CoteESRB</t>
   </si>
@@ -2488,6 +2488,9 @@
   </si>
   <si>
     <t>IdSysExp</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -3016,7 +3019,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -5644,10 +5647,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C46"/>
+  <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="M48" sqref="M48"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6027,6 +6030,11 @@
       </c>
       <c r="C46" s="13"/>
     </row>
+    <row r="54" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F54" t="s">
+        <v>819</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6037,7 +6045,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
maj script et JE erreur d'un theme en doublon
</commit_message>
<xml_diff>
--- a/Sprint 1/Package 1/Documentation/P01_JE_V2.xlsx
+++ b/Sprint 1/Package 1/Documentation/P01_JE_V2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="12228" yWindow="12" windowWidth="10800" windowHeight="9348" tabRatio="861" activeTab="12"/>
+    <workbookView xWindow="12228" yWindow="12" windowWidth="10800" windowHeight="9348" tabRatio="861" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="C tblSysExp" sheetId="3" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1182" uniqueCount="820">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1182" uniqueCount="821">
   <si>
     <t>CoteESRB</t>
   </si>
@@ -2491,6 +2491,9 @@
   </si>
   <si>
     <t>s</t>
+  </si>
+  <si>
+    <t>Lieu Caraïbes Plage</t>
   </si>
 </sst>
 </file>
@@ -3019,7 +3022,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -5649,7 +5652,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
@@ -6136,8 +6139,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C337"/>
   <sheetViews>
-    <sheetView topLeftCell="A325" workbookViewId="0">
-      <selection activeCell="C356" sqref="C356"/>
+    <sheetView tabSelected="1" topLeftCell="A181" workbookViewId="0">
+      <selection activeCell="B202" sqref="B202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7785,7 +7788,7 @@
         <v>202</v>
       </c>
       <c r="B203" t="s">
-        <v>368</v>
+        <v>820</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>